<commit_message>
Se crea clase para generar email aleatorio, se actualiza excel hoja createAccount y se actualiza flujo crear cuenta
</commit_message>
<xml_diff>
--- a/bin/test/data/Data.xlsx
+++ b/bin/test/data/Data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>functionality</t>
   </si>
@@ -181,9 +181,6 @@
     <t xml:space="preserve">Last Name</t>
   </si>
   <si>
-    <t xml:space="preserve">Email V</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -193,85 +190,13 @@
     <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">First Name2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Last Name2</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Address2</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
-    <t>PostalCode</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>AditionalIn</t>
-  </si>
-  <si>
-    <t>HomePhone</t>
-  </si>
-  <si>
-    <t>MobilePhone</t>
-  </si>
-  <si>
-    <t>Alias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email caso alterno</t>
-  </si>
-  <si>
-    <t>Mujer</t>
+    <t>Hombre</t>
   </si>
   <si>
     <t>Juan</t>
   </si>
   <si>
     <t>Osorio</t>
-  </si>
-  <si>
-    <t>juanp07@gmail.com</t>
-  </si>
-  <si>
-    <t>empresa</t>
-  </si>
-  <si>
-    <t>direccion2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apto 508</t>
-  </si>
-  <si>
-    <t>Bogota</t>
-  </si>
-  <si>
-    <t>Texas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States</t>
-  </si>
-  <si>
-    <t>Prueba1</t>
-  </si>
-  <si>
-    <t>juanpa</t>
-  </si>
-  <si>
-    <t>juanp006@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -284,7 +209,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -410,12 +335,6 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11.000000"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -918,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -953,9 +872,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf fontId="19" fillId="0" borderId="0" numFmtId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1893,14 +1809,11 @@
     <pageSetUpPr autoPageBreaks="1" fitToPage="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="100" workbookViewId="0">
       <selection activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8000000000000007" defaultRowHeight="14.25" outlineLevelRow="1"/>
-  <cols>
-    <col min="20" max="20" width="11.4"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1913,10 +1826,10 @@
         <v>53</v>
       </c>
       <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
         <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>28</v>
       </c>
       <c r="F1" t="s">
         <v>55</v>
@@ -1924,125 +1837,31 @@
       <c r="G1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
-      <c r="L1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" t="s">
-        <v>63</v>
-      </c>
-      <c r="O1" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>66</v>
-      </c>
-      <c r="R1" t="s">
-        <v>67</v>
-      </c>
-      <c r="S1" t="s">
-        <v>68</v>
-      </c>
-      <c r="T1" t="s">
-        <v>69</v>
-      </c>
-      <c r="U1" t="s">
-        <v>70</v>
-      </c>
-      <c r="V1" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" t="s">
         <v>31</v>
       </c>
+      <c r="E2">
+        <v>31</v>
+      </c>
       <c r="F2">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G2">
-        <v>3</v>
-      </c>
-      <c r="H2">
         <v>2000</v>
       </c>
-      <c r="I2" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L2" t="s">
-        <v>77</v>
-      </c>
-      <c r="M2" t="s">
-        <v>78</v>
-      </c>
-      <c r="N2" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" t="s">
-        <v>80</v>
-      </c>
-      <c r="P2">
-        <v>44444</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>81</v>
-      </c>
-      <c r="R2" t="s">
-        <v>82</v>
-      </c>
-      <c r="S2">
-        <v>7782696</v>
-      </c>
-      <c r="T2">
-        <v>3125049145</v>
-      </c>
-      <c r="U2" t="s">
-        <v>83</v>
-      </c>
-      <c r="V2" s="11" t="s">
-        <v>84</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink r:id="rId1" ref="D2"/>
-    <hyperlink r:id="rId2" ref="V2" tooltip="mailto:juanp006@gmail.com"/>
-  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>